<commit_message>
Clases para las R creadas
</commit_message>
<xml_diff>
--- a/Modulo 2/Reglas Gramaticales/Reglas.xlsx
+++ b/Modulo 2/Reglas Gramaticales/Reglas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumnoudg-my.sharepoint.com/personal/jorgea_zepeda_alumno_udg_mx/Documents/Universidad/6 Sexto/Seminario de traductores de lenguajes 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\52322\Desktop\QT-Traductor-Completo\Modulo 2\Reglas Gramaticales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="213" documentId="11_AD4D2F04E46CFB4ACB3E20323557E0DE693EDF17" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5CF335D-D579-48F7-A40B-3B599C9217F2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F658FA92-CCA9-48A3-9B29-ABD0099002CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="1275" windowWidth="15375" windowHeight="9540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -454,13 +454,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -748,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,7 +799,7 @@
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>58</v>
       </c>
       <c r="C3" s="2">
@@ -809,7 +809,7 @@
         <f t="shared" ref="D3:D53" si="0">C3*2</f>
         <v>0</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="13">
         <v>25</v>
       </c>
     </row>
@@ -817,7 +817,7 @@
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="14"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="2">
         <v>2</v>
       </c>
@@ -825,13 +825,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>59</v>
       </c>
       <c r="C5" s="2">
@@ -841,7 +841,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="13">
         <v>26</v>
       </c>
     </row>
@@ -849,7 +849,7 @@
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="14"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="2">
         <v>1</v>
       </c>
@@ -857,7 +857,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -881,7 +881,7 @@
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>61</v>
       </c>
       <c r="C8" s="2">
@@ -891,7 +891,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="13">
         <v>28</v>
       </c>
     </row>
@@ -899,7 +899,7 @@
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="14"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="2">
         <v>3</v>
       </c>
@@ -907,7 +907,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E9" s="12"/>
+      <c r="E9" s="13"/>
     </row>
     <row r="10" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
@@ -931,7 +931,7 @@
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="12" t="s">
         <v>63</v>
       </c>
       <c r="C11" s="2">
@@ -941,7 +941,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="13">
         <v>30</v>
       </c>
     </row>
@@ -949,7 +949,7 @@
       <c r="A12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="14"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="2">
         <v>3</v>
       </c>
@@ -957,13 +957,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E12" s="12"/>
+      <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C13" s="2">
@@ -973,7 +973,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="13">
         <v>31</v>
       </c>
     </row>
@@ -981,7 +981,7 @@
       <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="14"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="2">
         <v>4</v>
       </c>
@@ -989,7 +989,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E14" s="12"/>
+      <c r="E14" s="13"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -1013,7 +1013,7 @@
       <c r="A16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="12" t="s">
         <v>65</v>
       </c>
       <c r="C16" s="2">
@@ -1023,7 +1023,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="13">
         <v>33</v>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       <c r="A17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="14"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="2">
         <v>2</v>
       </c>
@@ -1039,13 +1039,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E17" s="12"/>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="12" t="s">
         <v>67</v>
       </c>
       <c r="C18" s="2">
@@ -1055,7 +1055,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="13">
         <v>34</v>
       </c>
     </row>
@@ -1063,7 +1063,7 @@
       <c r="A19" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="14"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="2">
         <v>1</v>
       </c>
@@ -1071,13 +1071,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E19" s="12"/>
+      <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="12" t="s">
         <v>68</v>
       </c>
       <c r="C20" s="2">
@@ -1095,7 +1095,7 @@
       <c r="A21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="14"/>
+      <c r="B21" s="12"/>
       <c r="C21" s="2">
         <v>2</v>
       </c>
@@ -1103,7 +1103,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="13">
         <v>36</v>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       <c r="A22" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="12" t="s">
         <v>78</v>
       </c>
       <c r="C22" s="2">
@@ -1121,13 +1121,13 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E22" s="12"/>
+      <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="14"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="2">
         <v>6</v>
       </c>
@@ -1135,13 +1135,13 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E23" s="12"/>
+      <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="14"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="2">
         <v>5</v>
       </c>
@@ -1149,13 +1149,13 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E24" s="12"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="14"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="2">
         <v>3</v>
       </c>
@@ -1163,13 +1163,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E25" s="12"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="14"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="2">
         <v>2</v>
       </c>
@@ -1177,13 +1177,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E26" s="12"/>
+      <c r="E26" s="13"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="12" t="s">
         <v>69</v>
       </c>
       <c r="C27" s="2">
@@ -1193,7 +1193,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="13">
         <v>37</v>
       </c>
     </row>
@@ -1201,7 +1201,7 @@
       <c r="A28" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="14"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="2">
         <v>2</v>
       </c>
@@ -1209,7 +1209,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E28" s="12"/>
+      <c r="E28" s="13"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
@@ -1233,7 +1233,7 @@
       <c r="A30" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="12" t="s">
         <v>71</v>
       </c>
       <c r="C30" s="2">
@@ -1243,7 +1243,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="13">
         <v>39</v>
       </c>
     </row>
@@ -1251,7 +1251,7 @@
       <c r="A31" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="14"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="2">
         <v>1</v>
       </c>
@@ -1259,13 +1259,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E31" s="12"/>
+      <c r="E31" s="13"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="12" t="s">
         <v>72</v>
       </c>
       <c r="C32" s="2">
@@ -1275,7 +1275,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="13">
         <v>40</v>
       </c>
     </row>
@@ -1283,7 +1283,7 @@
       <c r="A33" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="14"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="2">
         <v>2</v>
       </c>
@@ -1291,13 +1291,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E33" s="12"/>
+      <c r="E33" s="13"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="12" t="s">
         <v>73</v>
       </c>
       <c r="C34" s="2">
@@ -1307,7 +1307,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="13">
         <v>41</v>
       </c>
     </row>
@@ -1315,7 +1315,7 @@
       <c r="A35" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="14"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="2">
         <v>3</v>
       </c>
@@ -1323,13 +1323,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E35" s="12"/>
+      <c r="E35" s="13"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="12" t="s">
         <v>74</v>
       </c>
       <c r="C36" s="2">
@@ -1339,7 +1339,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E36" s="12">
+      <c r="E36" s="13">
         <v>42</v>
       </c>
     </row>
@@ -1347,7 +1347,7 @@
       <c r="A37" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="14"/>
+      <c r="B37" s="12"/>
       <c r="C37" s="2">
         <v>1</v>
       </c>
@@ -1355,13 +1355,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E37" s="12"/>
+      <c r="E37" s="13"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="14"/>
+      <c r="B38" s="12"/>
       <c r="C38" s="2">
         <v>1</v>
       </c>
@@ -1369,13 +1369,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E38" s="12"/>
+      <c r="E38" s="13"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="14"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="2">
         <v>1</v>
       </c>
@@ -1383,13 +1383,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E39" s="12"/>
+      <c r="E39" s="13"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="14"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="2">
         <v>1</v>
       </c>
@@ -1397,7 +1397,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E40" s="12"/>
+      <c r="E40" s="13"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
@@ -1421,7 +1421,7 @@
       <c r="A42" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="12" t="s">
         <v>76</v>
       </c>
       <c r="C42" s="2">
@@ -1431,7 +1431,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E42" s="12">
+      <c r="E42" s="13">
         <v>44</v>
       </c>
     </row>
@@ -1439,7 +1439,7 @@
       <c r="A43" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="14"/>
+      <c r="B43" s="12"/>
       <c r="C43" s="2">
         <v>1</v>
       </c>
@@ -1447,13 +1447,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E43" s="12"/>
+      <c r="E43" s="13"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="12" t="s">
         <v>77</v>
       </c>
       <c r="C44" s="2">
@@ -1463,7 +1463,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E44" s="12">
+      <c r="E44" s="13">
         <v>45</v>
       </c>
     </row>
@@ -1471,7 +1471,7 @@
       <c r="A45" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="14"/>
+      <c r="B45" s="12"/>
       <c r="C45" s="2">
         <v>2</v>
       </c>
@@ -1479,13 +1479,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E45" s="12"/>
+      <c r="E45" s="13"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B46" s="14"/>
+      <c r="B46" s="12"/>
       <c r="C46" s="2">
         <v>2</v>
       </c>
@@ -1493,13 +1493,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E46" s="12"/>
+      <c r="E46" s="13"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="14"/>
+      <c r="B47" s="12"/>
       <c r="C47" s="2">
         <v>3</v>
       </c>
@@ -1507,13 +1507,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E47" s="12"/>
+      <c r="E47" s="13"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="14"/>
+      <c r="B48" s="12"/>
       <c r="C48" s="2">
         <v>3</v>
       </c>
@@ -1521,13 +1521,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E48" s="12"/>
+      <c r="E48" s="13"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="14"/>
+      <c r="B49" s="12"/>
       <c r="C49" s="2">
         <v>3</v>
       </c>
@@ -1535,13 +1535,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E49" s="12"/>
+      <c r="E49" s="13"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="14"/>
+      <c r="B50" s="12"/>
       <c r="C50" s="2">
         <v>3</v>
       </c>
@@ -1549,13 +1549,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E50" s="12"/>
+      <c r="E50" s="13"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="14"/>
+      <c r="B51" s="12"/>
       <c r="C51" s="2">
         <v>3</v>
       </c>
@@ -1563,13 +1563,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E51" s="12"/>
+      <c r="E51" s="13"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="14"/>
+      <c r="B52" s="12"/>
       <c r="C52" s="2">
         <v>3</v>
       </c>
@@ -1577,7 +1577,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E52" s="12"/>
+      <c r="E52" s="13"/>
     </row>
     <row r="53" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
@@ -1591,26 +1591,10 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E53" s="13"/>
+      <c r="E53" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
     <mergeCell ref="E42:E43"/>
     <mergeCell ref="E44:E53"/>
     <mergeCell ref="B20:B21"/>
@@ -1626,6 +1610,22 @@
     <mergeCell ref="B44:B53"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="B34:B35"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>